<commit_message>
Excel Test data with Browser
</commit_message>
<xml_diff>
--- a/Framework/ExcelSheets/Sree.xlsx
+++ b/Framework/ExcelSheets/Sree.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schimbili\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schimbili\Documents\Visual Studio 2013\Projects\Framework-master\Framework-master\Framework\ExcelSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="240"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,12 +25,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Sreekanth</t>
-  </si>
-  <si>
-    <t>Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+  <si>
+    <t>Disney</t>
+  </si>
+  <si>
+    <t>WaltWhite</t>
+  </si>
+  <si>
+    <t>password1</t>
+  </si>
+  <si>
+    <t>CompanyId</t>
+  </si>
+  <si>
+    <t>inputID</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>sree</t>
+  </si>
+  <si>
+    <t>sree1</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
   </si>
 </sst>
 </file>
@@ -354,22 +379,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>